<commit_message>
Tested different solutions for setting the worker values.
</commit_message>
<xml_diff>
--- a/Graafikuseedija/src/Testing testing(1-24).xlsx
+++ b/Graafikuseedija/src/Testing testing(1-24).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f1f3b2b2e0b977bc/Documents/graafikuseedija/Graafikuseedija/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="13_ncr:1_{5300C98A-885F-4743-8A30-4A2DA5A71B1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1B75AF14-214D-4422-AA12-B9B26FFB642A}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="114_{E9E6BB18-2791-4407-A903-DDB38115B92D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0596B8D8-8510-4013-89AA-4ADA54EAEFE2}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="3465" yWindow="3465" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2370" yWindow="105" windowWidth="26085" windowHeight="13590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="44">
   <si>
     <t>ID</t>
   </si>
@@ -74,12 +74,6 @@
     <t>Sven-Ervin Paap</t>
   </si>
   <si>
-    <t>15-23</t>
-  </si>
-  <si>
-    <t>23-07</t>
-  </si>
-  <si>
     <t>23-07;</t>
   </si>
   <si>
@@ -170,10 +164,7 @@
     <t>Helena Jallai</t>
   </si>
   <si>
-    <t>07-15</t>
-  </si>
-  <si>
-    <t>Test</t>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -591,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -659,10 +650,10 @@
         <v>12</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -680,13 +671,13 @@
         <v>Taavi.Peeters@playtech.com</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -704,13 +695,13 @@
         <v>Siim.Lillemets@playtech.com</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -728,16 +719,16 @@
         <v>Joonas.Karl.Kuusik@playtech.com</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -755,25 +746,25 @@
         <v>Madis.Klesment@playtech.com</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -791,16 +782,16 @@
         <v>Daniell.Sepp@playtech.com</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -818,25 +809,28 @@
         <v>Helena.Mandel@playtech.com</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -854,16 +848,25 @@
         <v>Timo.Kirpu@playtech.com</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="I9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" s="3" t="s">
         <v>16</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -881,13 +884,13 @@
         <v>Deniz.Gülmez@playtech.com</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -905,19 +908,19 @@
         <v>Joel.Kikerpill@playtech.com</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -935,16 +938,16 @@
         <v>Anne-Mai.Pall@playtech.com</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -962,19 +965,19 @@
         <v>Martin.Merisalu@playtech.com</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K13" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -992,22 +995,22 @@
         <v>Rasmus.Rahnu@playtech.com</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1025,19 +1028,19 @@
         <v>Triinu.Saks@playtech.com</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J15" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1055,25 +1058,25 @@
         <v>Fred.Kasemaa@playtech.com</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -1091,19 +1094,19 @@
         <v>Robert.Matjus@playtech.com</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -1121,19 +1124,19 @@
         <v>Siim-Kaarel.Kabel@playtech.com</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -1151,10 +1154,13 @@
         <v>Siim-Sander.Sägi@playtech.com</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -1172,13 +1178,13 @@
         <v>Uku.Jaan.Leppik@playtech.com</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -1196,10 +1202,10 @@
         <v>Tanel.Madisson@playtech.com</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -1217,10 +1223,10 @@
         <v>Buse.Erdeem@playtech.com</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -1238,19 +1244,22 @@
         <v>Urmo.Olesk@playtech.com</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -1268,19 +1277,19 @@
         <v>Kevin.Vahtra@playtech.com</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -1298,28 +1307,25 @@
         <v>Helena.Jallai@playtech.com</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="L25" s="3" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed reading data from excel file
</commit_message>
<xml_diff>
--- a/Graafikuseedija/src/Testing testing(1-24).xlsx
+++ b/Graafikuseedija/src/Testing testing(1-24).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f1f3b2b2e0b977bc/Documents/graafikuseedija/Graafikuseedija/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="114_{E9E6BB18-2791-4407-A903-DDB38115B92D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0596B8D8-8510-4013-89AA-4ADA54EAEFE2}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="114_{E9E6BB18-2791-4407-A903-DDB38115B92D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BFEB1AAF-FC57-4A0E-8361-379C18444BB3}"/>
   <bookViews>
     <workbookView xWindow="2370" yWindow="105" windowWidth="26085" windowHeight="13590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="44">
   <si>
     <t>ID</t>
   </si>
@@ -582,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,6 +655,9 @@
       <c r="G2" s="3" t="s">
         <v>17</v>
       </c>
+      <c r="J2" s="3" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">

</xml_diff>

<commit_message>
Commented most of the code. Redid Graafikuseedija to include a GUI interface for choosing a file and save location. Modified README.md
</commit_message>
<xml_diff>
--- a/Graafikuseedija/src/Testing testing(1-24).xlsx
+++ b/Graafikuseedija/src/Testing testing(1-24).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f1f3b2b2e0b977bc/Documents/graafikuseedija/Graafikuseedija/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="114_{E9E6BB18-2791-4407-A903-DDB38115B92D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BFEB1AAF-FC57-4A0E-8361-379C18444BB3}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="114_{E9E6BB18-2791-4407-A903-DDB38115B92D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9D45ECBC-F4E3-4262-9B6E-F6BA7A50BFD2}"/>
   <bookViews>
-    <workbookView xWindow="2370" yWindow="105" windowWidth="26085" windowHeight="13590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3180" yWindow="300" windowWidth="23205" windowHeight="14550" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="21">
   <si>
     <t>ID</t>
   </si>
@@ -71,9 +71,6 @@
     <t>Pühapäev (22.03)</t>
   </si>
   <si>
-    <t>Sven-Ervin Paap</t>
-  </si>
-  <si>
     <t>23-07;</t>
   </si>
   <si>
@@ -95,76 +92,10 @@
     <t>07-15;15-23;</t>
   </si>
   <si>
-    <t>Taavi Peeters</t>
-  </si>
-  <si>
-    <t>Siim Lillemets</t>
-  </si>
-  <si>
-    <t>Joonas Karl Kuusik</t>
-  </si>
-  <si>
-    <t>Madis Klesment</t>
-  </si>
-  <si>
-    <t>Daniell Sepp</t>
-  </si>
-  <si>
-    <t>Helena Mandel</t>
-  </si>
-  <si>
-    <t>Timo Kirpu</t>
-  </si>
-  <si>
-    <t>Deniz Gülmez</t>
-  </si>
-  <si>
-    <t>Joel Kikerpill</t>
-  </si>
-  <si>
-    <t>Anne-Mai Pall</t>
-  </si>
-  <si>
-    <t>Martin Merisalu</t>
-  </si>
-  <si>
-    <t>Rasmus Rahnu</t>
-  </si>
-  <si>
-    <t>Triinu Saks</t>
-  </si>
-  <si>
-    <t>Fred Kasemaa</t>
-  </si>
-  <si>
-    <t>Robert Matjus</t>
-  </si>
-  <si>
-    <t>Siim-Kaarel Kabel</t>
-  </si>
-  <si>
-    <t>Siim-Sander Sägi</t>
-  </si>
-  <si>
-    <t>Uku Jaan Leppik</t>
-  </si>
-  <si>
-    <t>Tanel Madisson</t>
-  </si>
-  <si>
-    <t>Buse Erdeem</t>
-  </si>
-  <si>
-    <t>Urmo Olesk</t>
-  </si>
-  <si>
-    <t>Kevin Vahtra</t>
-  </si>
-  <si>
-    <t>Helena Jallai</t>
-  </si>
-  <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>?????</t>
   </si>
 </sst>
 </file>
@@ -583,7 +514,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,21 +573,18 @@
       <c r="C2" s="1">
         <v>43905.642476851797</v>
       </c>
-      <c r="D2" s="2" t="str">
-        <f>SUBSTITUTE(Table1[[#This Row],[Name]], " ", ".") &amp;  "@playtech.com"</f>
-        <v>Sven-Ervin.Paap@playtech.com</v>
-      </c>
+      <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -669,18 +597,15 @@
       <c r="C3" s="1">
         <v>43905.642800925903</v>
       </c>
-      <c r="D3" s="2" t="str">
-        <f>SUBSTITUTE(Table1[[#This Row],[Name]], " ", ".") &amp;  "@playtech.com"</f>
-        <v>Taavi.Peeters@playtech.com</v>
-      </c>
+      <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -693,18 +618,15 @@
       <c r="C4" s="1">
         <v>43905.642835648097</v>
       </c>
-      <c r="D4" s="2" t="str">
-        <f>SUBSTITUTE(Table1[[#This Row],[Name]], " ", ".") &amp;  "@playtech.com"</f>
-        <v>Siim.Lillemets@playtech.com</v>
-      </c>
+      <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -717,21 +639,18 @@
       <c r="C5" s="1">
         <v>43905.6843981481</v>
       </c>
-      <c r="D5" s="2" t="str">
-        <f>SUBSTITUTE(Table1[[#This Row],[Name]], " ", ".") &amp;  "@playtech.com"</f>
-        <v>Joonas.Karl.Kuusik@playtech.com</v>
-      </c>
+      <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -744,30 +663,27 @@
       <c r="C6" s="1">
         <v>43905.684502314798</v>
       </c>
-      <c r="D6" s="2" t="str">
-        <f>SUBSTITUTE(Table1[[#This Row],[Name]], " ", ".") &amp;  "@playtech.com"</f>
-        <v>Madis.Klesment@playtech.com</v>
-      </c>
+      <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -780,21 +696,18 @@
       <c r="C7" s="1">
         <v>43905.684583333299</v>
       </c>
-      <c r="D7" s="2" t="str">
-        <f>SUBSTITUTE(Table1[[#This Row],[Name]], " ", ".") &amp;  "@playtech.com"</f>
-        <v>Daniell.Sepp@playtech.com</v>
-      </c>
+      <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -807,33 +720,30 @@
       <c r="C8" s="1">
         <v>43905.684699074103</v>
       </c>
-      <c r="D8" s="2" t="str">
-        <f>SUBSTITUTE(Table1[[#This Row],[Name]], " ", ".") &amp;  "@playtech.com"</f>
-        <v>Helena.Mandel@playtech.com</v>
-      </c>
+      <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L8" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -846,30 +756,27 @@
       <c r="C9" s="1">
         <v>43905.684814814798</v>
       </c>
-      <c r="D9" s="2" t="str">
-        <f>SUBSTITUTE(Table1[[#This Row],[Name]], " ", ".") &amp;  "@playtech.com"</f>
-        <v>Timo.Kirpu@playtech.com</v>
-      </c>
+      <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -882,18 +789,15 @@
       <c r="C10" s="1">
         <v>43905.684895833299</v>
       </c>
-      <c r="D10" s="2" t="str">
-        <f>SUBSTITUTE(Table1[[#This Row],[Name]], " ", ".") &amp;  "@playtech.com"</f>
-        <v>Deniz.Gülmez@playtech.com</v>
-      </c>
+      <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -906,24 +810,21 @@
       <c r="C11" s="1">
         <v>43905.6850231481</v>
       </c>
-      <c r="D11" s="2" t="str">
-        <f>SUBSTITUTE(Table1[[#This Row],[Name]], " ", ".") &amp;  "@playtech.com"</f>
-        <v>Joel.Kikerpill@playtech.com</v>
-      </c>
+      <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -936,21 +837,18 @@
       <c r="C12" s="1">
         <v>43905.6852083333</v>
       </c>
-      <c r="D12" s="2" t="str">
-        <f>SUBSTITUTE(Table1[[#This Row],[Name]], " ", ".") &amp;  "@playtech.com"</f>
-        <v>Anne-Mai.Pall@playtech.com</v>
-      </c>
+      <c r="D12" s="2"/>
       <c r="E12" s="2" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K12" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -963,24 +861,21 @@
       <c r="C13" s="1">
         <v>43905.685347222199</v>
       </c>
-      <c r="D13" s="2" t="str">
-        <f>SUBSTITUTE(Table1[[#This Row],[Name]], " ", ".") &amp;  "@playtech.com"</f>
-        <v>Martin.Merisalu@playtech.com</v>
-      </c>
+      <c r="D13" s="2"/>
       <c r="E13" s="2" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -993,27 +888,24 @@
       <c r="C14" s="1">
         <v>43905.685856481497</v>
       </c>
-      <c r="D14" s="2" t="str">
-        <f>SUBSTITUTE(Table1[[#This Row],[Name]], " ", ".") &amp;  "@playtech.com"</f>
-        <v>Rasmus.Rahnu@playtech.com</v>
-      </c>
+      <c r="D14" s="2"/>
       <c r="E14" s="2" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1026,24 +918,21 @@
       <c r="C15" s="1">
         <v>43905.686041666697</v>
       </c>
-      <c r="D15" s="2" t="str">
-        <f>SUBSTITUTE(Table1[[#This Row],[Name]], " ", ".") &amp;  "@playtech.com"</f>
-        <v>Triinu.Saks@playtech.com</v>
-      </c>
+      <c r="D15" s="2"/>
       <c r="E15" s="2" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1056,30 +945,27 @@
       <c r="C16" s="1">
         <v>43905.686435185198</v>
       </c>
-      <c r="D16" s="2" t="str">
-        <f>SUBSTITUTE(Table1[[#This Row],[Name]], " ", ".") &amp;  "@playtech.com"</f>
-        <v>Fred.Kasemaa@playtech.com</v>
-      </c>
+      <c r="D16" s="2"/>
       <c r="E16" s="2" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -1092,24 +978,21 @@
       <c r="C17" s="1">
         <v>43905.687673611101</v>
       </c>
-      <c r="D17" s="2" t="str">
-        <f>SUBSTITUTE(Table1[[#This Row],[Name]], " ", ".") &amp;  "@playtech.com"</f>
-        <v>Robert.Matjus@playtech.com</v>
-      </c>
+      <c r="D17" s="2"/>
       <c r="E17" s="2" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -1122,24 +1005,21 @@
       <c r="C18" s="1">
         <v>43905.691562499997</v>
       </c>
-      <c r="D18" s="2" t="str">
-        <f>SUBSTITUTE(Table1[[#This Row],[Name]], " ", ".") &amp;  "@playtech.com"</f>
-        <v>Siim-Kaarel.Kabel@playtech.com</v>
-      </c>
+      <c r="D18" s="2"/>
       <c r="E18" s="2" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J18" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K18" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="K18" s="3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -1152,18 +1032,15 @@
       <c r="C19" s="1">
         <v>43905.691620370402</v>
       </c>
-      <c r="D19" s="2" t="str">
-        <f>SUBSTITUTE(Table1[[#This Row],[Name]], " ", ".") &amp;  "@playtech.com"</f>
-        <v>Siim-Sander.Sägi@playtech.com</v>
-      </c>
+      <c r="D19" s="2"/>
       <c r="E19" s="2" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -1176,18 +1053,15 @@
       <c r="C20" s="1">
         <v>43905.691724536999</v>
       </c>
-      <c r="D20" s="2" t="str">
-        <f>SUBSTITUTE(Table1[[#This Row],[Name]], " ", ".") &amp;  "@playtech.com"</f>
-        <v>Uku.Jaan.Leppik@playtech.com</v>
-      </c>
+      <c r="D20" s="2"/>
       <c r="E20" s="2" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -1200,15 +1074,12 @@
       <c r="C21" s="1">
         <v>43905.693495370397</v>
       </c>
-      <c r="D21" s="2" t="str">
-        <f>SUBSTITUTE(Table1[[#This Row],[Name]], " ", ".") &amp;  "@playtech.com"</f>
-        <v>Tanel.Madisson@playtech.com</v>
-      </c>
+      <c r="D21" s="2"/>
       <c r="E21" s="2" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -1221,15 +1092,12 @@
       <c r="C22" s="1">
         <v>43905.693564814799</v>
       </c>
-      <c r="D22" s="2" t="str">
-        <f>SUBSTITUTE(Table1[[#This Row],[Name]], " ", ".") &amp;  "@playtech.com"</f>
-        <v>Buse.Erdeem@playtech.com</v>
-      </c>
+      <c r="D22" s="2"/>
       <c r="E22" s="2" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -1242,27 +1110,24 @@
       <c r="C23" s="1">
         <v>43905.693981481498</v>
       </c>
-      <c r="D23" s="2" t="str">
-        <f>SUBSTITUTE(Table1[[#This Row],[Name]], " ", ".") &amp;  "@playtech.com"</f>
-        <v>Urmo.Olesk@playtech.com</v>
-      </c>
+      <c r="D23" s="2"/>
       <c r="E23" s="2" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -1275,24 +1140,21 @@
       <c r="C24" s="1">
         <v>43905.694305555597</v>
       </c>
-      <c r="D24" s="2" t="str">
-        <f>SUBSTITUTE(Table1[[#This Row],[Name]], " ", ".") &amp;  "@playtech.com"</f>
-        <v>Kevin.Vahtra@playtech.com</v>
-      </c>
+      <c r="D24" s="2"/>
       <c r="E24" s="2" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -1305,30 +1167,27 @@
       <c r="C25" s="1">
         <v>43905.694432870398</v>
       </c>
-      <c r="D25" s="2" t="str">
-        <f>SUBSTITUTE(Table1[[#This Row],[Name]], " ", ".") &amp;  "@playtech.com"</f>
-        <v>Helena.Jallai@playtech.com</v>
-      </c>
+      <c r="D25" s="2"/>
       <c r="E25" s="2" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New GUI class for interacting with the user.
</commit_message>
<xml_diff>
--- a/Graafikuseedija/src/Testing testing(1-24).xlsx
+++ b/Graafikuseedija/src/Testing testing(1-24).xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="14" documentId="114_{E9E6BB18-2791-4407-A903-DDB38115B92D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9D45ECBC-F4E3-4262-9B6E-F6BA7A50BFD2}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="300" windowWidth="23205" windowHeight="14550" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2655" yWindow="705" windowWidth="23205" windowHeight="14550" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -514,7 +514,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>